<commit_message>
Update SRS Document: Screen flow of Admin
</commit_message>
<xml_diff>
--- a/Document/Product_Backlog.xlsx
+++ b/Document/Product_Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Kì 5\SWP391\Project\Week 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Kì 5\SWP391\ShopOnline\ShopOnlineThunderBolt\ShoppingOnlineThunderbolt\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B13AFF-8CD5-4215-A1C8-D00FA5C9C5A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3076069-A062-4467-8DB5-F2F932F33E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DF743DC6-3E10-FC40-A74C-7ADFA9B03788}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="55">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -194,15 +194,6 @@
   </si>
   <si>
     <t>My Orders (xem lịch sử order) (tổng quát)</t>
-  </si>
-  <si>
-    <t>now</t>
-  </si>
-  <si>
-    <t>noow</t>
-  </si>
-  <si>
-    <t>done</t>
   </si>
 </sst>
 </file>
@@ -832,8 +823,8 @@
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1226,9 +1217,7 @@
       <c r="D28" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
     </row>
@@ -1245,9 +1234,7 @@
       <c r="D29" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
     </row>
@@ -1264,9 +1251,7 @@
       <c r="D30" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
     </row>
@@ -1283,9 +1268,7 @@
       <c r="D31" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
@@ -1302,9 +1285,7 @@
       <c r="D32" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="7" t="s">
-        <v>56</v>
-      </c>
+      <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
     </row>
@@ -1321,9 +1302,7 @@
       <c r="D33" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
     </row>
@@ -1409,9 +1388,7 @@
         <v>8</v>
       </c>
       <c r="E38" s="7"/>
-      <c r="F38" s="7" t="s">
-        <v>57</v>
-      </c>
+      <c r="F38" s="7"/>
       <c r="G38" s="7"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -1461,9 +1438,7 @@
       <c r="D41" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E41" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
     </row>

</xml_diff>

<commit_message>
Update ProductBacklog: Work Division for this week and Status (Done or not) of all Screens
</commit_message>
<xml_diff>
--- a/Document/Product_Backlog.xlsx
+++ b/Document/Product_Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Kì 5\SWP391\ShopOnline\ShopOnlineThunderBolt\ShoppingOnlineThunderbolt\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3076069-A062-4467-8DB5-F2F932F33E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24825F35-63B1-4945-A267-8704725529D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DF743DC6-3E10-FC40-A74C-7ADFA9B03788}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$D$1:$D$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$D$1:$D$42</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="68">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -178,12 +178,6 @@
     <t>User Details</t>
   </si>
   <si>
-    <t>Settings List</t>
-  </si>
-  <si>
-    <t>Setting Details</t>
-  </si>
-  <si>
     <t>Cart Contact (List Cart)</t>
   </si>
   <si>
@@ -194,6 +188,51 @@
   </si>
   <si>
     <t>My Orders (xem lịch sử order) (tổng quát)</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Đang</t>
+  </si>
+  <si>
+    <t>Còn feedback</t>
+  </si>
+  <si>
+    <t>Còn Style</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>Khi bấm vào 1 User trong List -&gt; hiển thị chi tiết</t>
+  </si>
+  <si>
+    <t>Còn Paging</t>
+  </si>
+  <si>
+    <t>(Là Manager Product)</t>
+  </si>
+  <si>
+    <t>Hỏi Thuận: Total Invoices có chưa (nếu chưa có thì thêm 1 trang nữa)</t>
+  </si>
+  <si>
+    <t>cx thế</t>
+  </si>
+  <si>
+    <t>Sửa lại trang Total Invoices</t>
+  </si>
+  <si>
+    <t>Cx thế</t>
+  </si>
+  <si>
+    <t>Danh sách các Blog do Seller tạo ra</t>
+  </si>
+  <si>
+    <t>Chỉ có Seller Post thôi</t>
+  </si>
+  <si>
+    <t>Slot sau hỏi thầy</t>
   </si>
 </sst>
 </file>
@@ -270,7 +309,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +364,18 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -358,7 +409,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -420,6 +471,8 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -821,10 +874,10 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -836,10 +889,12 @@
     <col min="5" max="5" width="11.44140625" customWidth="1"/>
     <col min="6" max="6" width="17.77734375" customWidth="1"/>
     <col min="7" max="7" width="10.77734375" customWidth="1"/>
-    <col min="8" max="229" width="8.77734375" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" customWidth="1"/>
+    <col min="10" max="229" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="9"/>
       <c r="B1" s="8"/>
       <c r="C1" s="9"/>
@@ -848,7 +903,7 @@
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9"/>
       <c r="B2" s="8"/>
       <c r="C2" s="9"/>
@@ -857,7 +912,7 @@
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="8"/>
       <c r="C3" s="9"/>
@@ -866,7 +921,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="9"/>
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
@@ -875,7 +930,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7" ht="19.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="12" t="s">
         <v>0</v>
@@ -886,7 +941,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="11" t="s">
         <v>11</v>
@@ -897,7 +952,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="10"/>
       <c r="B7" s="8"/>
       <c r="C7" s="9"/>
@@ -906,7 +961,7 @@
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -928,104 +983,178 @@
       <c r="G8" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="6"/>
+      <c r="H8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>6</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="H9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="19" t="s">
+      <c r="H10" s="27"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>16</v>
       </c>
+      <c r="C11" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="C15" s="20" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D15" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="22" t="s">
-        <v>7</v>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="D16" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>7</v>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="D17" s="21" t="s">
         <v>6</v>
@@ -1033,16 +1162,20 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>7</v>
+      <c r="H17" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>5</v>
       </c>
       <c r="D18" s="21" t="s">
         <v>6</v>
@@ -1050,13 +1183,17 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>16</v>
+      <c r="H18" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>46</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>5</v>
@@ -1067,149 +1204,177 @@
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>6</v>
+      <c r="H19" s="28"/>
+      <c r="I19" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" s="23" t="s">
+      <c r="H20" s="27"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>6</v>
+      <c r="C21" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="24" t="s">
+      <c r="H21" s="27"/>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>6</v>
+      <c r="C22" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>6</v>
+      <c r="H22" s="27"/>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="21" t="s">
-        <v>6</v>
+      <c r="H23" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>6</v>
+      <c r="H24" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="21" t="s">
-        <v>6</v>
+      <c r="H25" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>6</v>
+      <c r="H26" s="27"/>
+      <c r="I26" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>8</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>16</v>
+      <c r="H27" s="27"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="C28" s="25" t="s">
         <v>5</v>
@@ -1220,13 +1385,17 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H28" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C29" s="25" t="s">
         <v>5</v>
@@ -1237,13 +1406,17 @@
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H29" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C30" s="25" t="s">
         <v>5</v>
@@ -1254,13 +1427,15 @@
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H30" s="27"/>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="C31" s="25" t="s">
         <v>5</v>
@@ -1271,13 +1446,17 @@
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="18" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C32" s="25" t="s">
         <v>5</v>
@@ -1288,13 +1467,17 @@
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" s="18" t="s">
-        <v>30</v>
+      <c r="H32" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>16</v>
       </c>
       <c r="C33" s="25" t="s">
         <v>5</v>
@@ -1305,149 +1488,175 @@
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="17" t="s">
-        <v>8</v>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="7"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>8</v>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36" s="18" t="s">
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>8</v>
+      <c r="C36" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="18" t="s">
+      <c r="H36" s="27"/>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C37" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>8</v>
+      <c r="C37" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="17" t="s">
-        <v>8</v>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>8</v>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
       <c r="G39" s="7"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>8</v>
+      <c r="H39" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>8</v>
+      <c r="H40" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>10</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
       <c r="G41" s="7"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>16</v>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="C42" s="26" t="s">
         <v>5</v>
@@ -1458,156 +1667,23 @@
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B43" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-      <c r="G43" s="7"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B44" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="B45" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B46" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C46" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C47" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="7"/>
-      <c r="F47" s="7"/>
-      <c r="G47" s="7"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-    </row>
-    <row r="49" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="B50" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="7"/>
-      <c r="F50" s="7"/>
-      <c r="G50" s="7"/>
-    </row>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="49" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="D1:D50" xr:uid="{3D2E7A14-9B86-4191-9515-6C47420033E4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:D50">
-    <sortCondition ref="D50"/>
+  <autoFilter ref="D1:D42" xr:uid="{3D2E7A14-9B86-4191-9515-6C47420033E4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:D42">
+    <sortCondition ref="D42"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G16" xr:uid="{DD16DB9A-416B-F24E-A930-C955FCC74FAE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10 C13:C42" xr:uid="{D8E3F485-0609-C341-A723-993F74FF62FF}">
+      <formula1>"Simple, Medium, Complex"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G10" xr:uid="{DD16DB9A-416B-F24E-A930-C955FCC74FAE}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3, Final"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C16 C44:C50 C19:C43" xr:uid="{D8E3F485-0609-C341-A723-993F74FF62FF}">
-      <formula1>"Simple, Medium, Complex"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D44:D50 D9:D43" xr:uid="{F07339E9-D44D-8E47-91D9-ADD73292BB26}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D42" xr:uid="{F07339E9-D44D-8E47-91D9-ADD73292BB26}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update Product Backlog: Contribution Percent
</commit_message>
<xml_diff>
--- a/Document/Product_Backlog.xlsx
+++ b/Document/Product_Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Kì 5\SWP391\ShopOnline\ShopOnlineThunderBolt\ShoppingOnlineThunderbolt\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Kì 5\SWP391\Project\Week 8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B5F35D-4009-4881-A952-F68FD201C504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F2BA2C-1EA2-4572-A9EB-03D21EE423B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DF743DC6-3E10-FC40-A74C-7ADFA9B03788}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$D$1:$D$42</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="95">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -184,6 +184,99 @@
     <t>Status</t>
   </si>
   <si>
+    <t>User Authorization</t>
+  </si>
+  <si>
+    <t>Cart Completion (Place Order)</t>
+  </si>
+  <si>
+    <t>HE153046, HE150346</t>
+  </si>
+  <si>
+    <t>HE153046</t>
+  </si>
+  <si>
+    <t>HE150411, HE150346</t>
+  </si>
+  <si>
+    <t>HE153046, HE150340</t>
+  </si>
+  <si>
+    <t>HE153590</t>
+  </si>
+  <si>
+    <t>HE150411, HE153590</t>
+  </si>
+  <si>
+    <t>HE150340</t>
+  </si>
+  <si>
+    <t>Notification</t>
+  </si>
+  <si>
+    <t>Compare Product</t>
+  </si>
+  <si>
+    <t>HE153046, HE150346, HE153590</t>
+  </si>
+  <si>
+    <t>HE153046, HE150346, HE150411, HE153590</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>BE: Back-end</t>
+  </si>
+  <si>
+    <t>FE: Front-end</t>
+  </si>
+  <si>
+    <t>Nguyen The Giang(BE-50), Bui Ngoc Huyen(FE-50)</t>
+  </si>
+  <si>
+    <t>Nguyen The Giang(BE-70), Bui Ngoc Huyen(FE-30)</t>
+  </si>
+  <si>
+    <t>HE153046, HE150346, HE153590, HE150411</t>
+  </si>
+  <si>
+    <t>Nguyen The Giang(BE-20), Bui Ngoc Huyen(FE-40), Dinh The Thuan(BE-20), Tran Tat Dat(BE-20)</t>
+  </si>
+  <si>
+    <t>Nguyen The Giang(BE-30), Bui Ngoc Huyen(FE-40, BE-20), Dinh The Thuan(BE-10)</t>
+  </si>
+  <si>
+    <t>Nguyen The Giang(BE-50), Phung Quang Thong(BE-50)</t>
+  </si>
+  <si>
+    <t>Nguyen The Giang(BE-25), Bui Ngoc Huyen(FE-25), Tran Tat Dat(BE-25), Dinh The Thuan(BE-25)</t>
+  </si>
+  <si>
+    <t>Tran Tat Dat(BE-50), Bui Ngoc Huyen(FE-50)</t>
+  </si>
+  <si>
+    <t>Tran Tat Dat(BE,FE-50), Dinh The Thuan(BE,FE-50)</t>
+  </si>
+  <si>
+    <t>Tran Tat Dat(BE-70), Phung Quang Thong(BE-20),Bui Ngoc Huyen(FE-10)</t>
+  </si>
+  <si>
+    <t>HE150411, HE150340,HE150346</t>
+  </si>
+  <si>
+    <t>Nguyen The Giang(BE-50, FE-50)</t>
+  </si>
+  <si>
+    <t>Phung Quang Thong(BE-50, FE-50)</t>
+  </si>
+  <si>
+    <t>Dinh The Thuan(BE-50, FE-50)</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
     <t>Đang</t>
   </si>
   <si>
@@ -193,18 +286,18 @@
     <t>Còn Style</t>
   </si>
   <si>
-    <t>Detail</t>
+    <t>Còn Paging</t>
   </si>
   <si>
     <t>Khi bấm vào 1 User trong List -&gt; hiển thị chi tiết</t>
   </si>
   <si>
-    <t>Còn Paging</t>
-  </si>
-  <si>
     <t>(Là Manager Product)</t>
   </si>
   <si>
+    <t>Khi bấm vào thì hiển thị Product Detail như User</t>
+  </si>
+  <si>
     <t>Hỏi Thuận: Total Invoices có chưa (nếu chưa có thì thêm 1 trang nữa)</t>
   </si>
   <si>
@@ -217,70 +310,10 @@
     <t>Cx thế</t>
   </si>
   <si>
+    <t>Chỉ có Seller Post thôi</t>
+  </si>
+  <si>
     <t>Danh sách các Blog do Seller tạo ra</t>
-  </si>
-  <si>
-    <t>Chỉ có Seller Post thôi</t>
-  </si>
-  <si>
-    <t>Dinh The Thuan</t>
-  </si>
-  <si>
-    <t>Nguyen The Giang</t>
-  </si>
-  <si>
-    <t>Tran Tat Dat, Dinh The Thuan</t>
-  </si>
-  <si>
-    <t>Khi bấm vào thì hiển thị Product Detail như User</t>
-  </si>
-  <si>
-    <t>User Authorization</t>
-  </si>
-  <si>
-    <t>Nguyen The Giang, Bui Ngoc Huyen</t>
-  </si>
-  <si>
-    <t>Tran Tat Dat, Bui Ngoc Huyen</t>
-  </si>
-  <si>
-    <t>Cart Completion (Place Order)</t>
-  </si>
-  <si>
-    <t>Nguyen The Giang, Bui Ngoc Huyen, Tran Tat Dat</t>
-  </si>
-  <si>
-    <t>Nguyen The Giang, Phung Quang Thong</t>
-  </si>
-  <si>
-    <t>Tran Tat Dat, Phung Quang Thong</t>
-  </si>
-  <si>
-    <t>HE153046, HE150346</t>
-  </si>
-  <si>
-    <t>HE153046</t>
-  </si>
-  <si>
-    <t>HE150411, HE150346</t>
-  </si>
-  <si>
-    <t>HE153046, HE150340</t>
-  </si>
-  <si>
-    <t>HE150411, HE150340</t>
-  </si>
-  <si>
-    <t>HE153590</t>
-  </si>
-  <si>
-    <t>HE150411, HE153590</t>
-  </si>
-  <si>
-    <t>HE150340</t>
-  </si>
-  <si>
-    <t>Phung Quang Thong</t>
   </si>
 </sst>
 </file>
@@ -369,7 +402,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,6 +481,12 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -481,7 +520,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -557,14 +596,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="5" xr:uid="{17DD364F-74B1-4D8B-8617-F9200D6E3605}"/>
-    <cellStyle name="Normal 3" xfId="3" xr:uid="{32FF9B6C-0366-4A77-B0D6-25B6DD3BFF75}"/>
-    <cellStyle name="Normal 5" xfId="2" xr:uid="{962DD808-D234-E447-A3DA-EC3FA1D4FD3F}"/>
-    <cellStyle name="Percent 2" xfId="4" xr:uid="{EE585932-6F1A-4B5F-A2D6-E1C450CB953E}"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 5" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Percent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -954,28 +994,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7C6098-9A84-DF47-8776-29A23ED803E4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I49"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.77734375" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="10.109375" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" customWidth="1"/>
-    <col min="6" max="6" width="44.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="10.44140625" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.44140625" customWidth="1"/>
+    <col min="6" max="6" width="79.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
     <col min="8" max="8" width="15.88671875" customWidth="1"/>
-    <col min="9" max="9" width="22.88671875" customWidth="1"/>
-    <col min="10" max="229" width="8.77734375" customWidth="1"/>
+    <col min="9" max="9" width="42.5546875" customWidth="1"/>
+    <col min="10" max="227" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -1071,7 +1111,7 @@
         <v>50</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>54</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1091,7 +1131,7 @@
       <c r="F9" s="32"/>
       <c r="G9" s="4"/>
       <c r="H9" s="5" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="I9" s="5"/>
     </row>
@@ -1109,10 +1149,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="24"/>
@@ -1126,20 +1166,20 @@
         <v>16</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -1157,10 +1197,10 @@
         <v>6</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="24"/>
@@ -1174,16 +1214,16 @@
         <v>16</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D13" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="24"/>
@@ -1197,16 +1237,16 @@
         <v>24</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="24"/>
@@ -1220,16 +1260,16 @@
         <v>24</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F15" s="34" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="24"/>
@@ -1237,22 +1277,22 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="31" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="B16" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E16" s="33" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="F16" s="33" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="24"/>
@@ -1266,20 +1306,20 @@
         <v>44</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="F17" s="34" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -1291,20 +1331,20 @@
         <v>44</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>6</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="F18" s="34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="25" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="I18" s="5"/>
     </row>
@@ -1326,27 +1366,27 @@
       <c r="G19" s="5"/>
       <c r="H19" s="25"/>
       <c r="I19" s="5" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="14" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B20" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="24"/>
@@ -1366,10 +1406,10 @@
         <v>8</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="24"/>
@@ -1383,16 +1423,16 @@
         <v>24</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="24"/>
@@ -1406,20 +1446,20 @@
         <v>24</v>
       </c>
       <c r="C23" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="I23" s="5"/>
     </row>
@@ -1431,20 +1471,20 @@
         <v>29</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E24" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="33" t="s">
         <v>80</v>
-      </c>
-      <c r="F24" s="33" t="s">
-        <v>64</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="I24" s="5"/>
     </row>
@@ -1456,20 +1496,20 @@
         <v>29</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D25" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="F25" s="33" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="I25" s="5"/>
     </row>
@@ -1481,21 +1521,21 @@
         <v>31</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="G26" s="5"/>
       <c r="H26" s="24"/>
       <c r="I26" s="5" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1516,7 +1556,7 @@
       <c r="G27" s="5"/>
       <c r="H27" s="25"/>
       <c r="I27" s="5" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1527,20 +1567,20 @@
         <v>31</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F28" s="33" t="s">
         <v>80</v>
-      </c>
-      <c r="F28" s="33" t="s">
-        <v>64</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="I28" s="5"/>
     </row>
@@ -1558,14 +1598,14 @@
         <v>8</v>
       </c>
       <c r="E29" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29" s="33" t="s">
         <v>80</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>64</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="5" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="I29" s="5"/>
     </row>
@@ -1583,10 +1623,10 @@
         <v>8</v>
       </c>
       <c r="E30" s="35" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="F30" s="34" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="24"/>
@@ -1600,20 +1640,20 @@
         <v>31</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F31" s="33" t="s">
         <v>80</v>
-      </c>
-      <c r="F31" s="33" t="s">
-        <v>64</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="I31" s="5"/>
     </row>
@@ -1625,20 +1665,20 @@
         <v>31</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="33" t="s">
         <v>80</v>
-      </c>
-      <c r="F32" s="33" t="s">
-        <v>64</v>
       </c>
       <c r="G32" s="5"/>
       <c r="H32" s="5" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="I32" s="5"/>
     </row>
@@ -1650,16 +1690,16 @@
         <v>16</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
@@ -1673,21 +1713,21 @@
         <v>16</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
       <c r="I34" s="5" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -1704,10 +1744,10 @@
         <v>10</v>
       </c>
       <c r="E35" s="33" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="F35" s="33" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
@@ -1750,7 +1790,7 @@
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -1848,20 +1888,81 @@
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
     </row>
-    <row r="49" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B43" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C43" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F43" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F44" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F46" s="37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F47" s="37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F48" s="37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="D1:D42" xr:uid="{3D2E7A14-9B86-4191-9515-6C47420033E4}"/>
+  <autoFilter ref="D1:D42" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:D42">
     <sortCondition ref="D42"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10 C13:C42" xr:uid="{D8E3F485-0609-C341-A723-993F74FF62FF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10 C13:C44" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Simple, Medium, Complex"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G10" xr:uid="{DD16DB9A-416B-F24E-A930-C955FCC74FAE}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3, Final"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D42" xr:uid="{F07339E9-D44D-8E47-91D9-ADD73292BB26}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D44" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update Product Backlog; Update Table [Blog] in Database; Add Data to Table [Blog]
</commit_message>
<xml_diff>
--- a/Document/Product_Backlog.xlsx
+++ b/Document/Product_Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Kì 5\SWP391\Project\Week 8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Kì 5\SWP391\ShopOnline\ShopOnlineThunderBolt\ShoppingOnlineThunderbolt\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F2BA2C-1EA2-4572-A9EB-03D21EE423B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78412A46-04B8-42ED-A547-F8AD730F5B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$D$1:$D$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$D$1:$D$41</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="95">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -172,9 +172,6 @@
     <t>User Details</t>
   </si>
   <si>
-    <t>Cart Contact (List Cart)</t>
-  </si>
-  <si>
     <t>Order Information (chi tiết)</t>
   </si>
   <si>
@@ -314,6 +311,9 @@
   </si>
   <si>
     <t>Danh sách các Blog do Seller tạo ra</t>
+  </si>
+  <si>
+    <t>Đã xóa trong SRS (vì nó ko tồn tại)</t>
   </si>
 </sst>
 </file>
@@ -324,7 +324,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -400,6 +400,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="15">
@@ -520,7 +527,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -597,6 +604,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -998,10 +1006,10 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I51"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27:F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1108,10 +1116,10 @@
         <v>4</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1131,7 +1139,7 @@
       <c r="F9" s="32"/>
       <c r="G9" s="4"/>
       <c r="H9" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I9" s="5"/>
     </row>
@@ -1149,10 +1157,10 @@
         <v>6</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="24"/>
@@ -1172,14 +1180,14 @@
         <v>6</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -1197,21 +1205,21 @@
         <v>6</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="24"/>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>16</v>
+      <c r="A13" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>24</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>9</v>
@@ -1220,10 +1228,10 @@
         <v>6</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="24"/>
@@ -1231,7 +1239,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>24</v>
@@ -1243,138 +1251,140 @@
         <v>6</v>
       </c>
       <c r="E14" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="34" t="s">
         <v>69</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>70</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="24"/>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="21" t="s">
+      <c r="A15" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="31" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>70</v>
+      <c r="E15" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>78</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="24"/>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="31" t="s">
-        <v>24</v>
+      <c r="A16" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>44</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>79</v>
+      <c r="E16" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>70</v>
       </c>
       <c r="G16" s="5"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="5"/>
+      <c r="H16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="I16" s="38" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B17" s="21" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D17" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="35" t="s">
-        <v>62</v>
+      <c r="E17" s="33" t="s">
+        <v>55</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>71</v>
       </c>
       <c r="G17" s="5"/>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="25" t="s">
         <v>84</v>
       </c>
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" s="21" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="33" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="34" t="s">
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="G18" s="5"/>
-      <c r="H18" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="I18" s="5"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="33"/>
-      <c r="F19" s="33"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="5" t="s">
-        <v>86</v>
-      </c>
+      <c r="H19" s="24"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>16</v>
+      <c r="A20" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="C20" s="22" t="s">
         <v>9</v>
@@ -1383,10 +1393,10 @@
         <v>8</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="24"/>
@@ -1394,22 +1404,22 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="34" t="s">
-        <v>67</v>
+      <c r="E21" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>73</v>
       </c>
       <c r="G21" s="5"/>
       <c r="H21" s="24"/>
@@ -1417,7 +1427,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B22" s="16" t="s">
         <v>24</v>
@@ -1429,21 +1439,23 @@
         <v>8</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F22" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G22" s="5"/>
-      <c r="H22" s="24"/>
+      <c r="H22" s="5" t="s">
+        <v>83</v>
+      </c>
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C23" s="22" t="s">
         <v>7</v>
@@ -1452,20 +1464,20 @@
         <v>8</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F23" s="33" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>29</v>
@@ -1480,20 +1492,20 @@
         <v>57</v>
       </c>
       <c r="F24" s="33" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>7</v>
@@ -1502,81 +1514,81 @@
         <v>8</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="F25" s="33" t="s">
-        <v>75</v>
+        <v>53</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>77</v>
       </c>
       <c r="G25" s="5"/>
-      <c r="H25" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="I25" s="5"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C26" s="22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D26" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="34" t="s">
-        <v>78</v>
-      </c>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="24"/>
+      <c r="H26" s="25"/>
       <c r="I26" s="5" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B27" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C27" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D27" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
+      <c r="E27" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>79</v>
+      </c>
       <c r="G27" s="5"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="5" t="s">
+      <c r="H27" s="5" t="s">
         <v>88</v>
       </c>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F28" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5" t="s">
@@ -1586,35 +1598,33 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B29" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C29" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D29" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>80</v>
+      <c r="E29" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" s="34" t="s">
+        <v>66</v>
       </c>
       <c r="G29" s="5"/>
-      <c r="H29" s="5" t="s">
-        <v>90</v>
-      </c>
+      <c r="H29" s="24"/>
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C30" s="22" t="s">
         <v>7</v>
@@ -1622,19 +1632,21 @@
       <c r="D30" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="35" t="s">
-        <v>53</v>
-      </c>
-      <c r="F30" s="34" t="s">
-        <v>67</v>
+      <c r="E30" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F30" s="33" t="s">
+        <v>79</v>
       </c>
       <c r="G30" s="5"/>
-      <c r="H30" s="24"/>
+      <c r="H30" s="5" t="s">
+        <v>90</v>
+      </c>
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B31" s="16" t="s">
         <v>31</v>
@@ -1646,10 +1658,10 @@
         <v>8</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F31" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5" t="s">
@@ -1658,123 +1670,119 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="16" t="s">
-        <v>31</v>
+      <c r="A32" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="C32" s="22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D32" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="33" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="F32" s="33" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G32" s="5"/>
-      <c r="H32" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="H32" s="5"/>
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="14" t="s">
+      <c r="A33" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>8</v>
+      <c r="C33" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>10</v>
       </c>
       <c r="E33" s="33" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="F33" s="33" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
+      <c r="I33" s="5" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D34" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E34" s="33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F34" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="5" t="s">
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="29"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B35" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="33" t="s">
-        <v>59</v>
-      </c>
-      <c r="F35" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-    </row>
-    <row r="36" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="29"/>
-      <c r="I36" s="29"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B37" s="13" t="s">
         <v>31</v>
@@ -1789,32 +1797,30 @@
       <c r="F37" s="33"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="13" t="s">
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
     </row>
     <row r="39" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B39" s="26" t="s">
         <v>31</v>
@@ -1831,28 +1837,28 @@
       <c r="H39" s="29"/>
       <c r="I39" s="29"/>
     </row>
-    <row r="40" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B40" s="26" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D40" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
-      <c r="H40" s="29"/>
-      <c r="I40" s="29"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B41" s="13" t="s">
         <v>31</v>
@@ -1871,10 +1877,10 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C42" s="23" t="s">
         <v>5</v>
@@ -1882,8 +1888,12 @@
       <c r="D42" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
+      <c r="E42" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="F42" s="33" t="s">
+        <v>79</v>
+      </c>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
@@ -1893,46 +1903,28 @@
         <v>60</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>10</v>
       </c>
       <c r="E43" s="33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F43" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C44" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="F44" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F45" s="37" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F46" s="37" t="s">
@@ -1944,25 +1936,20 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F48" s="37" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="51" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="D1:D42" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:D42">
-    <sortCondition ref="D42"/>
+  <autoFilter ref="D1:D41" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:D41">
+    <sortCondition ref="D41"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10 C13:C44" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10 C13:C43" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Simple, Medium, Complex"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3, Final"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D44" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D43" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update SRS Document & Product Backlog
</commit_message>
<xml_diff>
--- a/Document/Product_Backlog.xlsx
+++ b/Document/Product_Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Kì 5\SWP391\ShopOnline\ShopOnlineThunderBolt\ShoppingOnlineThunderbolt\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E43FE37-C907-4689-B3DF-578B8DA0D290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2257BAB-5766-46F9-8C3F-D2F263913087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="95">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -307,13 +307,13 @@
     <t>Cx thế</t>
   </si>
   <si>
-    <t>Chỉ có Seller Post thôi</t>
-  </si>
-  <si>
-    <t>Danh sách các Blog do Seller tạo ra</t>
-  </si>
-  <si>
     <t>Đã xóa trong SRS (vì nó ko tồn tại)</t>
+  </si>
+  <si>
+    <t>HE150411</t>
+  </si>
+  <si>
+    <t>Tran Tat Dat(BE-50, FE-50)</t>
   </si>
 </sst>
 </file>
@@ -1008,8 +1008,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1307,7 +1307,7 @@
         <v>83</v>
       </c>
       <c r="I16" s="38" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1713,9 +1713,7 @@
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
-      <c r="I33" s="5" t="s">
-        <v>92</v>
-      </c>
+      <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
@@ -1772,13 +1770,15 @@
       <c r="D36" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="33"/>
-      <c r="F36" s="33"/>
+      <c r="E36" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="33" t="s">
+        <v>78</v>
+      </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="5" t="s">
-        <v>93</v>
-      </c>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
@@ -1793,8 +1793,12 @@
       <c r="D37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="33"/>
-      <c r="F37" s="33"/>
+      <c r="E37" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>78</v>
+      </c>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
@@ -1850,8 +1854,12 @@
       <c r="D40" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="33"/>
-      <c r="F40" s="33"/>
+      <c r="E40" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F40" s="33" t="s">
+        <v>94</v>
+      </c>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
@@ -1869,8 +1877,12 @@
       <c r="D41" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="33"/>
-      <c r="F41" s="33"/>
+      <c r="E41" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="33" t="s">
+        <v>94</v>
+      </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>

</xml_diff>

<commit_message>
Update Product Backlog: Contributor for Home Page
</commit_message>
<xml_diff>
--- a/Document/Product_Backlog.xlsx
+++ b/Document/Product_Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Kì 5\SWP391\ShopOnline\ShopOnlineThunderBolt\ShoppingOnlineThunderbolt\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2257BAB-5766-46F9-8C3F-D2F263913087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F356872B-2003-4402-B047-2D162D104C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="94">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -272,9 +272,6 @@
   </si>
   <si>
     <t>Detail</t>
-  </si>
-  <si>
-    <t>Đang</t>
   </si>
   <si>
     <t>Còn feedback</t>
@@ -527,7 +524,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -598,7 +595,6 @@
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="5" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1008,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1135,12 +1131,14 @@
       <c r="D9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>77</v>
+      </c>
       <c r="G9" s="4"/>
-      <c r="H9" s="5" t="s">
-        <v>81</v>
-      </c>
+      <c r="H9" s="24"/>
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1156,10 +1154,10 @@
       <c r="D10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="F10" s="33" t="s">
         <v>66</v>
       </c>
       <c r="G10" s="4"/>
@@ -1179,15 +1177,15 @@
       <c r="D11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="33" t="s">
+      <c r="E11" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="F11" s="33" t="s">
         <v>77</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I11" s="5"/>
     </row>
@@ -1204,10 +1202,10 @@
       <c r="D12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="34" t="s">
+      <c r="F12" s="33" t="s">
         <v>67</v>
       </c>
       <c r="G12" s="5"/>
@@ -1227,10 +1225,10 @@
       <c r="D13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="33" t="s">
         <v>69</v>
       </c>
       <c r="G13" s="5"/>
@@ -1250,10 +1248,10 @@
       <c r="D14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="33" t="s">
         <v>69</v>
       </c>
       <c r="G14" s="5"/>
@@ -1273,10 +1271,10 @@
       <c r="D15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="32" t="s">
         <v>78</v>
       </c>
       <c r="G15" s="5"/>
@@ -1296,18 +1294,18 @@
       <c r="D16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F16" s="33" t="s">
         <v>70</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I16" s="38" t="s">
-        <v>92</v>
+        <v>82</v>
+      </c>
+      <c r="I16" s="37" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1323,15 +1321,15 @@
       <c r="D17" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="F17" s="34" t="s">
+      <c r="F17" s="33" t="s">
         <v>71</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I17" s="5"/>
     </row>
@@ -1348,12 +1346,12 @@
       <c r="D18" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
       <c r="G18" s="5"/>
       <c r="H18" s="25"/>
       <c r="I18" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1369,10 +1367,10 @@
       <c r="D19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="F19" s="33" t="s">
         <v>72</v>
       </c>
       <c r="G19" s="5"/>
@@ -1392,10 +1390,10 @@
       <c r="D20" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="F20" s="33" t="s">
         <v>66</v>
       </c>
       <c r="G20" s="5"/>
@@ -1415,10 +1413,10 @@
       <c r="D21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="33" t="s">
+      <c r="F21" s="32" t="s">
         <v>73</v>
       </c>
       <c r="G21" s="5"/>
@@ -1438,15 +1436,15 @@
       <c r="D22" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="33" t="s">
+      <c r="F22" s="32" t="s">
         <v>73</v>
       </c>
       <c r="G22" s="5"/>
       <c r="H22" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I22" s="5"/>
     </row>
@@ -1463,15 +1461,15 @@
       <c r="D23" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F23" s="33" t="s">
+      <c r="F23" s="32" t="s">
         <v>79</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I23" s="5"/>
     </row>
@@ -1488,15 +1486,15 @@
       <c r="D24" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="F24" s="33" t="s">
+      <c r="F24" s="32" t="s">
         <v>74</v>
       </c>
       <c r="G24" s="5"/>
       <c r="H24" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I24" s="5"/>
     </row>
@@ -1513,16 +1511,16 @@
       <c r="D25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="34" t="s">
+      <c r="F25" s="33" t="s">
         <v>77</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="24"/>
       <c r="I25" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1538,12 +1536,12 @@
       <c r="D26" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="33"/>
-      <c r="F26" s="33"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
       <c r="G26" s="5"/>
       <c r="H26" s="25"/>
       <c r="I26" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1559,15 +1557,15 @@
       <c r="D27" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="32" t="s">
         <v>79</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I27" s="5"/>
     </row>
@@ -1584,15 +1582,15 @@
       <c r="D28" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F28" s="33" t="s">
+      <c r="F28" s="32" t="s">
         <v>79</v>
       </c>
       <c r="G28" s="5"/>
       <c r="H28" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I28" s="5"/>
     </row>
@@ -1609,10 +1607,10 @@
       <c r="D29" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="F29" s="34" t="s">
+      <c r="F29" s="33" t="s">
         <v>66</v>
       </c>
       <c r="G29" s="5"/>
@@ -1632,15 +1630,15 @@
       <c r="D30" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="33" t="s">
+      <c r="E30" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="33" t="s">
+      <c r="F30" s="32" t="s">
         <v>79</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I30" s="5"/>
     </row>
@@ -1657,15 +1655,15 @@
       <c r="D31" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="32" t="s">
         <v>79</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I31" s="5"/>
     </row>
@@ -1682,10 +1680,10 @@
       <c r="D32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="33" t="s">
+      <c r="E32" s="32" t="s">
         <v>76</v>
       </c>
-      <c r="F32" s="33" t="s">
+      <c r="F32" s="32" t="s">
         <v>75</v>
       </c>
       <c r="G32" s="5"/>
@@ -1705,10 +1703,10 @@
       <c r="D33" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="33" t="s">
+      <c r="E33" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="33" t="s">
+      <c r="F33" s="32" t="s">
         <v>78</v>
       </c>
       <c r="G33" s="5"/>
@@ -1728,10 +1726,10 @@
       <c r="D34" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="E34" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="F34" s="33" t="s">
+      <c r="F34" s="32" t="s">
         <v>78</v>
       </c>
       <c r="G34" s="5"/>
@@ -1752,7 +1750,7 @@
         <v>10</v>
       </c>
       <c r="E35" s="29"/>
-      <c r="F35" s="36"/>
+      <c r="F35" s="35"/>
       <c r="G35" s="29"/>
       <c r="H35" s="29"/>
       <c r="I35" s="29"/>
@@ -1770,10 +1768,10 @@
       <c r="D36" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="33" t="s">
+      <c r="E36" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="F36" s="33" t="s">
+      <c r="F36" s="32" t="s">
         <v>78</v>
       </c>
       <c r="G36" s="5"/>
@@ -1793,10 +1791,10 @@
       <c r="D37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="33" t="s">
+      <c r="E37" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="F37" s="33" t="s">
+      <c r="F37" s="32" t="s">
         <v>78</v>
       </c>
       <c r="G37" s="5"/>
@@ -1854,11 +1852,11 @@
       <c r="D40" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="33" t="s">
+      <c r="E40" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F40" s="32" t="s">
         <v>93</v>
-      </c>
-      <c r="F40" s="33" t="s">
-        <v>94</v>
       </c>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
@@ -1877,11 +1875,11 @@
       <c r="D41" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="33" t="s">
+      <c r="E41" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="32" t="s">
         <v>93</v>
-      </c>
-      <c r="F41" s="33" t="s">
-        <v>94</v>
       </c>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
@@ -1900,10 +1898,10 @@
       <c r="D42" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="33" t="s">
+      <c r="E42" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F42" s="33" t="s">
+      <c r="F42" s="32" t="s">
         <v>79</v>
       </c>
       <c r="G42" s="5"/>
@@ -1923,10 +1921,10 @@
       <c r="D43" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E43" s="33" t="s">
+      <c r="E43" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="F43" s="33" t="s">
+      <c r="F43" s="32" t="s">
         <v>79</v>
       </c>
       <c r="G43" s="5"/>
@@ -1934,17 +1932,17 @@
       <c r="I43" s="5"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F45" s="37" t="s">
+      <c r="F45" s="36" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F46" s="37" t="s">
+      <c r="F46" s="36" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F47" s="37" t="s">
+      <c r="F47" s="36" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Product Backlog: Finish
</commit_message>
<xml_diff>
--- a/Document/Product_Backlog.xlsx
+++ b/Document/Product_Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Kì 5\SWP391\ShopOnline\ShopOnlineThunderBolt\ShoppingOnlineThunderbolt\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADC204E-2B7D-4BB6-9390-9AC1B05C94C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4872F1-ADBA-44B1-BEBB-843BB3795DC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$D$1:$D$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Product Backlog'!$D$1:$D$36</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="79">
   <si>
     <t>THE APPLICATION DEVELOPMENT PROJECT TOPIC</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Customer</t>
   </si>
   <si>
-    <t>MKT Dashboard</t>
-  </si>
-  <si>
     <t>Marketing</t>
   </si>
   <si>
@@ -133,12 +130,6 @@
     <t>Post Details</t>
   </si>
   <si>
-    <t>Sliders List</t>
-  </si>
-  <si>
-    <t>Slider Details</t>
-  </si>
-  <si>
     <t>Customers List</t>
   </si>
   <si>
@@ -169,18 +160,12 @@
     <t>Users List</t>
   </si>
   <si>
-    <t>User Details</t>
-  </si>
-  <si>
     <t>Order Information (chi tiết)</t>
   </si>
   <si>
     <t>My Orders (xem lịch sử order) (tổng quát)</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>User Authorization</t>
   </si>
   <si>
@@ -271,46 +256,16 @@
     <t>Dinh The Thuan(BE-50, FE-50)</t>
   </si>
   <si>
-    <t>Detail</t>
-  </si>
-  <si>
-    <t>Còn feedback</t>
-  </si>
-  <si>
-    <t>Còn Style</t>
-  </si>
-  <si>
-    <t>Còn Paging</t>
-  </si>
-  <si>
-    <t>Khi bấm vào 1 User trong List -&gt; hiển thị chi tiết</t>
-  </si>
-  <si>
-    <t>(Là Manager Product)</t>
-  </si>
-  <si>
-    <t>Khi bấm vào thì hiển thị Product Detail như User</t>
-  </si>
-  <si>
-    <t>Hỏi Thuận: Total Invoices có chưa (nếu chưa có thì thêm 1 trang nữa)</t>
-  </si>
-  <si>
-    <t>cx thế</t>
-  </si>
-  <si>
-    <t>Sửa lại trang Total Invoices</t>
-  </si>
-  <si>
-    <t>Cx thế</t>
-  </si>
-  <si>
-    <t>Đã xóa trong SRS (vì nó ko tồn tại)</t>
-  </si>
-  <si>
     <t>HE150411</t>
   </si>
   <si>
     <t>Tran Tat Dat(BE-50, FE-50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iteration 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iteration 3</t>
   </si>
 </sst>
 </file>
@@ -321,7 +276,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,31 +337,11 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="0" tint="-0.499984740745262"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="15">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -463,30 +398,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -524,7 +435,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -581,26 +492,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="5" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="12" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="5" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="5" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1002,10 +900,10 @@
   <sheetPr>
     <outlinePr summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -1017,12 +915,10 @@
     <col min="5" max="5" width="38.44140625" customWidth="1"/>
     <col min="6" max="6" width="79.5546875" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
-    <col min="9" max="9" width="42.5546875" customWidth="1"/>
-    <col min="10" max="227" width="8.6640625" customWidth="1"/>
+    <col min="8" max="225" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
       <c r="B1" s="6"/>
       <c r="C1" s="7"/>
@@ -1031,7 +927,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
@@ -1040,7 +936,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
@@ -1049,7 +945,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="6"/>
       <c r="C4" s="7"/>
@@ -1058,7 +954,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="19.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="10" t="s">
         <v>0</v>
@@ -1069,7 +965,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
       <c r="B6" s="9" t="s">
         <v>11</v>
@@ -1080,7 +976,7 @@
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="6"/>
       <c r="C7" s="7"/>
@@ -1089,7 +985,7 @@
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
-    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1111,14 +1007,8 @@
       <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>15</v>
       </c>
@@ -1131,17 +1021,17 @@
       <c r="D9" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E9" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="17" t="s">
         <v>19</v>
       </c>
@@ -1154,17 +1044,17 @@
       <c r="D10" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E10" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="17" t="s">
         <v>20</v>
       </c>
@@ -1177,19 +1067,17 @@
       <c r="D11" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E11" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="17" t="s">
         <v>21</v>
       </c>
@@ -1202,17 +1090,17 @@
       <c r="D12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="33" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E12" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>23</v>
       </c>
@@ -1225,17 +1113,17 @@
       <c r="D13" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" s="5"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E13" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
         <v>25</v>
       </c>
@@ -1248,21 +1136,21 @@
       <c r="D14" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E14" s="34" t="s">
-        <v>68</v>
-      </c>
-      <c r="F14" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="5"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="31" t="s">
+      <c r="E14" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="24" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="18" t="s">
@@ -1271,22 +1159,22 @@
       <c r="D15" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="5"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E15" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="21" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>9</v>
@@ -1294,26 +1182,22 @@
       <c r="D16" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="33" t="s">
-        <v>70</v>
-      </c>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I16" s="37" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E16" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C17" s="18" t="s">
         <v>7</v>
@@ -1321,45 +1205,45 @@
       <c r="D17" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="E17" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>71</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="25" t="s">
-        <v>83</v>
-      </c>
-      <c r="I17" s="5"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="21" t="s">
+      <c r="E17" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="14" t="s">
+      <c r="B18" s="14" t="s">
         <v>16</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="C19" s="22" t="s">
         <v>9</v>
@@ -1367,42 +1251,42 @@
       <c r="D19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E19" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="5"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E19" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E20" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="5"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E20" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>24</v>
@@ -1413,22 +1297,22 @@
       <c r="D21" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E21" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G21" s="5"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="5"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E21" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>7</v>
@@ -1436,21 +1320,19 @@
       <c r="D22" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="F22" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I22" s="5"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E22" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>29</v>
@@ -1461,24 +1343,22 @@
       <c r="D23" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E23" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E23" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C24" s="22" t="s">
         <v>7</v>
@@ -1486,24 +1366,22 @@
       <c r="D24" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E24" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="I24" s="5"/>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E24" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="22" t="s">
         <v>7</v>
@@ -1511,24 +1389,22 @@
       <c r="D25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="F25" s="33" t="s">
+      <c r="E25" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G25" s="5"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C26" s="22" t="s">
         <v>5</v>
@@ -1536,20 +1412,22 @@
       <c r="D26" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="5" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E26" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="22" t="s">
         <v>7</v>
@@ -1557,49 +1435,45 @@
       <c r="D27" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E27" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="I27" s="5"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E27" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C28" s="22" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D28" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E28" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="F28" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="I28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E28" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="22" t="s">
         <v>7</v>
@@ -1607,118 +1481,114 @@
       <c r="D29" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="F29" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="5"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>44</v>
+      <c r="E29" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>16</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="I30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31" s="16" t="s">
+      <c r="E30" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F31" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="I31" s="5"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C32" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="F32" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>16</v>
+      <c r="B33" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D33" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="F33" s="32" t="s">
+      <c r="E33" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="11" t="s">
-        <v>16</v>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="C34" s="23" t="s">
         <v>5</v>
@@ -1726,41 +1596,45 @@
       <c r="D34" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="F34" s="32" t="s">
+      <c r="E34" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="G34" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-    </row>
-    <row r="35" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="26" t="s">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="35"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E35" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C36" s="23" t="s">
         <v>5</v>
@@ -1768,22 +1642,22 @@
       <c r="D36" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="F36" s="32" t="s">
+      <c r="E36" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C37" s="23" t="s">
         <v>5</v>
@@ -1791,175 +1665,68 @@
       <c r="D37" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="32" t="s">
+      <c r="E37" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F38" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F40" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="F37" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
-      <c r="H38" s="29"/>
-      <c r="I38" s="29"/>
-    </row>
-    <row r="39" spans="1:9" s="30" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29"/>
-      <c r="G39" s="29"/>
-      <c r="H39" s="29"/>
-      <c r="I39" s="29"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C40" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="F40" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="13" t="s">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F41" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C42" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="F42" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="13" t="s">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F42" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C43" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D43" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="F43" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F45" s="36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F46" s="36" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="F47" s="36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="50" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    </row>
+    <row r="45" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <autoFilter ref="D1:D41" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:D41">
-    <sortCondition ref="D41"/>
+  <autoFilter ref="D1:D36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A9:D36">
+    <sortCondition ref="D36"/>
   </sortState>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10 C13:C43" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C10 C13:C38" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Simple, Medium, Complex"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G10" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G9:G17" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3, Final"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D43" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D38" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Iteration 1, Iteration 2, Iteration 3"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>